<commit_message>
Parse personal business listings
</commit_message>
<xml_diff>
--- a/xlsx/general_abbreviation_list.xlsx
+++ b/xlsx/general_abbreviation_list.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="304">
   <si>
     <t>al</t>
   </si>
@@ -281,12 +281,6 @@
     <t>Public School</t>
   </si>
   <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>roomer</t>
-  </si>
-  <si>
     <t>rd</t>
   </si>
   <si>
@@ -347,24 +341,6 @@
     <t>United States</t>
   </si>
   <si>
-    <t>USA</t>
-  </si>
-  <si>
-    <t>United States Army</t>
-  </si>
-  <si>
-    <t>USMC</t>
-  </si>
-  <si>
-    <t>United States Marine Corps</t>
-  </si>
-  <si>
-    <t>USN</t>
-  </si>
-  <si>
-    <t>United States Navy</t>
-  </si>
-  <si>
     <t>West</t>
   </si>
   <si>
@@ -410,15 +386,6 @@
     <t>trav</t>
   </si>
   <si>
-    <t>transportation</t>
-  </si>
-  <si>
-    <t>trans</t>
-  </si>
-  <si>
-    <t>transp</t>
-  </si>
-  <si>
     <t>telephone</t>
   </si>
   <si>
@@ -501,12 +468,6 @@
   </si>
   <si>
     <t>ret</t>
-  </si>
-  <si>
-    <t>restaurant</t>
-  </si>
-  <si>
-    <t>restr</t>
   </si>
   <si>
     <t>refrigerator</t>
@@ -1347,10 +1308,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B164"/>
+  <dimension ref="A1:B157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
+      <selection activeCell="A147" sqref="A146:XFD147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1360,34 +1321,34 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="B1" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="B2" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="B3" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="B4" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1416,18 +1377,18 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="B8" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="B9" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1464,18 +1425,18 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="B14" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B15" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -1488,10 +1449,10 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
       <c r="B17" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -1504,10 +1465,10 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="B19" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -1536,10 +1497,10 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="B23" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -1552,18 +1513,18 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="B25" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="B26" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -1576,18 +1537,18 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="B28" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="B29" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -1616,18 +1577,18 @@
     </row>
     <row r="33" spans="1:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c r="B33" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c r="B34" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1640,26 +1601,26 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B36" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="B37" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="B38" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -1667,7 +1628,7 @@
         <v>32</v>
       </c>
       <c r="B39" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -1680,10 +1641,10 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="B41" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -1696,34 +1657,34 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="B43" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="B44" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="B45" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="B46" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -1744,42 +1705,42 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="B49" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="B50" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="B51" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="B52" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="B53" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -1792,34 +1753,34 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="B55" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="B56" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="B57" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="B58" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -1832,18 +1793,18 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="B60" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="B61" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
@@ -1856,58 +1817,58 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="B63" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="B64" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="B65" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="B66" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="B67" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="B68" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="B69" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
@@ -1928,34 +1889,34 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="B72" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="B73" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="B74" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="B75" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
@@ -1968,42 +1929,42 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="B77" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="B78" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="B79" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="B80" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="B81" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
@@ -2016,18 +1977,18 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="B83" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
       <c r="B84" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
@@ -2040,34 +2001,34 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="B86" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="B87" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="B88" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="B89" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
@@ -2080,26 +2041,26 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="B91" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="B92" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="B93" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
@@ -2152,10 +2113,10 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="B100" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
@@ -2208,18 +2169,18 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="B107" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="B108" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
@@ -2227,39 +2188,39 @@
         <v>83</v>
       </c>
       <c r="B109" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="B110" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="B111" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="B112" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="B113" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
@@ -2272,314 +2233,314 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="B115" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="B116" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="B117" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="B118" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="B119" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="B120" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="B121" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="B122" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="B123" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="B124" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>159</v>
+        <v>86</v>
       </c>
       <c r="B125" t="s">
-        <v>158</v>
+        <v>87</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>88</v>
+        <v>146</v>
       </c>
       <c r="B126" t="s">
-        <v>89</v>
+        <v>145</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>157</v>
+        <v>88</v>
       </c>
       <c r="B127" t="s">
-        <v>156</v>
+        <v>89</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>86</v>
+        <v>144</v>
       </c>
       <c r="B128" t="s">
-        <v>87</v>
+        <v>143</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>90</v>
+        <v>142</v>
       </c>
       <c r="B129" t="s">
-        <v>91</v>
+        <v>141</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="B130" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="B131" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="B132" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="B133" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="B134" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>145</v>
+        <v>91</v>
       </c>
       <c r="B135" t="s">
-        <v>144</v>
+        <v>90</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>143</v>
+        <v>92</v>
       </c>
       <c r="B136" t="s">
-        <v>142</v>
+        <v>93</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B137" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B138" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>96</v>
+        <v>130</v>
       </c>
       <c r="B139" t="s">
-        <v>97</v>
+        <v>129</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
       <c r="B140" t="s">
-        <v>99</v>
+        <v>127</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="B141" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="B142" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="B143" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>135</v>
+        <v>98</v>
       </c>
       <c r="B144" t="s">
-        <v>134</v>
+        <v>99</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>133</v>
+        <v>100</v>
       </c>
       <c r="B145" t="s">
-        <v>132</v>
+        <v>101</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="B146" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="B147" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>131</v>
+        <v>104</v>
       </c>
       <c r="B148" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>130</v>
+        <v>102</v>
       </c>
       <c r="B149" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>128</v>
+        <v>286</v>
       </c>
       <c r="B150" t="s">
-        <v>127</v>
+        <v>287</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>126</v>
+        <v>298</v>
       </c>
       <c r="B151" t="s">
-        <v>125</v>
+        <v>299</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B152" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B153" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
@@ -2592,87 +2553,31 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>112</v>
+        <v>288</v>
       </c>
       <c r="B155" t="s">
-        <v>113</v>
+        <v>289</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>104</v>
+        <v>290</v>
       </c>
       <c r="B156" t="s">
-        <v>105</v>
+        <v>291</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="B157" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A158" t="s">
-        <v>311</v>
-      </c>
-      <c r="B158" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A159" t="s">
-        <v>116</v>
-      </c>
-      <c r="B159" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A160" t="s">
-        <v>115</v>
-      </c>
-      <c r="B160" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A161" t="s">
-        <v>118</v>
-      </c>
-      <c r="B161" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A162" t="s">
-        <v>301</v>
-      </c>
-      <c r="B162" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A163" t="s">
-        <v>303</v>
-      </c>
-      <c r="B163" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A164" t="s">
-        <v>305</v>
-      </c>
-      <c r="B164" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:B164">
-    <sortCondition ref="B1"/>
+  <sortState ref="A1:B157">
+    <sortCondition ref="B123"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>